<commit_message>
Actualizacion de las HU, HT, PB, SB
</commit_message>
<xml_diff>
--- a/Documents/HU, HT, PB, SB.xlsx
+++ b/Documents/HU, HT, PB, SB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ff47571d30268be/Documentos/6/APLICACIONE II/Proyecto/SIGDCOLTA/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9E2EBF68-07CF-4AFC-AA75-7B7F2117A3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C5C59B7-1F09-4D4E-859A-4AAE39DF41E9}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9E2EBF68-07CF-4AFC-AA75-7B7F2117A3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73C3792F-E1A4-4730-92DD-D98E3BE22DDD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="9" xr2:uid="{D7927580-9A21-4766-84F0-58BE9C7E4DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="8" xr2:uid="{D7927580-9A21-4766-84F0-58BE9C7E4DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="RF y RNF" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="828">
   <si>
     <t>Identificador (ID) de la Historia</t>
   </si>
@@ -3450,174 +3450,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3660,6 +3492,174 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4610,7 +4610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7319D34E-C980-405C-B005-218F4118AF08}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -4620,24 +4620,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="191" t="s">
         <v>568</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="192" t="s">
         <v>569</v>
       </c>
-      <c r="C1" s="175" t="s">
+      <c r="C1" s="193" t="s">
         <v>604</v>
       </c>
-      <c r="D1" s="174" t="s">
+      <c r="D1" s="192" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="173"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="174"/>
+      <c r="A2" s="191"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="194"/>
+      <c r="D2" s="192"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="38" t="s">
@@ -4717,7 +4717,7 @@
       <c r="A10" s="137" t="s">
         <v>615</v>
       </c>
-      <c r="B10" s="232">
+      <c r="B10" s="176">
         <v>45272</v>
       </c>
       <c r="C10" s="137" t="s">
@@ -4772,32 +4772,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="191" t="s">
         <v>568</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="192" t="s">
         <v>569</v>
       </c>
-      <c r="C1" s="175" t="s">
+      <c r="C1" s="193" t="s">
         <v>580</v>
       </c>
-      <c r="D1" s="175" t="s">
+      <c r="D1" s="193" t="s">
         <v>738</v>
       </c>
-      <c r="E1" s="175" t="s">
+      <c r="E1" s="193" t="s">
         <v>739</v>
       </c>
-      <c r="F1" s="174" t="s">
+      <c r="F1" s="192" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="173"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="174"/>
+      <c r="A2" s="191"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="194"/>
+      <c r="D2" s="194"/>
+      <c r="E2" s="194"/>
+      <c r="F2" s="192"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="141" t="s">
@@ -4916,20 +4916,20 @@
   <sheetData>
     <row r="1" spans="1:11" ht="45.75" customHeight="1">
       <c r="A1" s="154"/>
-      <c r="B1" s="191" t="s">
+      <c r="B1" s="209" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="192"/>
-      <c r="D1" s="192"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
       <c r="E1" s="152"/>
       <c r="F1" s="152"/>
       <c r="G1" s="153"/>
-      <c r="H1" s="181" t="s">
+      <c r="H1" s="203" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="182"/>
-      <c r="J1" s="182"/>
-      <c r="K1" s="183"/>
+      <c r="I1" s="204"/>
+      <c r="J1" s="204"/>
+      <c r="K1" s="205"/>
     </row>
     <row r="2" spans="1:11" ht="45.75" customHeight="1">
       <c r="A2" s="155" t="s">
@@ -4968,11 +4968,11 @@
     </row>
     <row r="3" spans="1:11" ht="45.75" customHeight="1">
       <c r="A3" s="35"/>
-      <c r="B3" s="180" t="s">
+      <c r="B3" s="202" t="s">
         <v>782</v>
       </c>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
       <c r="E3" s="131"/>
       <c r="F3" s="131"/>
       <c r="G3" s="36"/>
@@ -4982,22 +4982,22 @@
       <c r="K3" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A4" s="184" t="s">
+      <c r="A4" s="201" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="185" t="s">
+      <c r="B4" s="195" t="s">
         <v>462</v>
       </c>
-      <c r="C4" s="185" t="s">
+      <c r="C4" s="195" t="s">
         <v>463</v>
       </c>
-      <c r="D4" s="185" t="s">
+      <c r="D4" s="195" t="s">
         <v>464</v>
       </c>
-      <c r="E4" s="177" t="s">
+      <c r="E4" s="198" t="s">
         <v>791</v>
       </c>
-      <c r="F4" s="177" t="s">
+      <c r="F4" s="198" t="s">
         <v>758</v>
       </c>
       <c r="G4" s="40">
@@ -5017,12 +5017,12 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A5" s="184"/>
-      <c r="B5" s="186"/>
-      <c r="C5" s="186"/>
-      <c r="D5" s="186"/>
-      <c r="E5" s="178"/>
-      <c r="F5" s="178"/>
+      <c r="A5" s="201"/>
+      <c r="B5" s="196"/>
+      <c r="C5" s="196"/>
+      <c r="D5" s="196"/>
+      <c r="E5" s="199"/>
+      <c r="F5" s="199"/>
       <c r="G5" s="40">
         <v>2</v>
       </c>
@@ -5040,12 +5040,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A6" s="184"/>
-      <c r="B6" s="187"/>
-      <c r="C6" s="187"/>
-      <c r="D6" s="187"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179"/>
+      <c r="A6" s="201"/>
+      <c r="B6" s="197"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="200"/>
       <c r="G6" s="128">
         <v>3</v>
       </c>
@@ -5056,11 +5056,11 @@
     </row>
     <row r="7" spans="1:11" ht="45.75" customHeight="1">
       <c r="A7" s="27"/>
-      <c r="B7" s="188" t="s">
+      <c r="B7" s="206" t="s">
         <v>783</v>
       </c>
-      <c r="C7" s="189"/>
-      <c r="D7" s="190"/>
+      <c r="C7" s="207"/>
+      <c r="D7" s="208"/>
       <c r="E7" s="132"/>
       <c r="F7" s="132"/>
       <c r="G7" s="27"/>
@@ -5070,22 +5070,22 @@
       <c r="K7" s="28"/>
     </row>
     <row r="8" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A8" s="184" t="s">
+      <c r="A8" s="201" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="185" t="s">
+      <c r="B8" s="195" t="s">
         <v>465</v>
       </c>
-      <c r="C8" s="185" t="s">
+      <c r="C8" s="195" t="s">
         <v>466</v>
       </c>
-      <c r="D8" s="185" t="s">
+      <c r="D8" s="195" t="s">
         <v>467</v>
       </c>
-      <c r="E8" s="177" t="s">
+      <c r="E8" s="198" t="s">
         <v>792</v>
       </c>
-      <c r="F8" s="177" t="s">
+      <c r="F8" s="198" t="s">
         <v>758</v>
       </c>
       <c r="G8" s="40">
@@ -5105,12 +5105,12 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A9" s="184"/>
-      <c r="B9" s="186"/>
-      <c r="C9" s="186"/>
-      <c r="D9" s="186"/>
-      <c r="E9" s="178"/>
-      <c r="F9" s="178"/>
+      <c r="A9" s="201"/>
+      <c r="B9" s="196"/>
+      <c r="C9" s="196"/>
+      <c r="D9" s="196"/>
+      <c r="E9" s="199"/>
+      <c r="F9" s="199"/>
       <c r="G9" s="34">
         <v>2</v>
       </c>
@@ -5128,12 +5128,12 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A10" s="184"/>
-      <c r="B10" s="187"/>
-      <c r="C10" s="187"/>
-      <c r="D10" s="187"/>
-      <c r="E10" s="179"/>
-      <c r="F10" s="179"/>
+      <c r="A10" s="201"/>
+      <c r="B10" s="197"/>
+      <c r="C10" s="197"/>
+      <c r="D10" s="197"/>
+      <c r="E10" s="200"/>
+      <c r="F10" s="200"/>
       <c r="G10" s="128">
         <v>3</v>
       </c>
@@ -5144,11 +5144,11 @@
     </row>
     <row r="11" spans="1:11" ht="45.75" customHeight="1">
       <c r="A11" s="35"/>
-      <c r="B11" s="180" t="s">
+      <c r="B11" s="202" t="s">
         <v>371</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="180"/>
+      <c r="C11" s="202"/>
+      <c r="D11" s="202"/>
       <c r="E11" s="151"/>
       <c r="F11" s="151"/>
       <c r="G11" s="35"/>
@@ -5158,22 +5158,22 @@
       <c r="K11" s="36"/>
     </row>
     <row r="12" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A12" s="184" t="s">
+      <c r="A12" s="201" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="185" t="s">
+      <c r="B12" s="195" t="s">
         <v>468</v>
       </c>
-      <c r="C12" s="185" t="s">
+      <c r="C12" s="195" t="s">
         <v>469</v>
       </c>
-      <c r="D12" s="185" t="s">
+      <c r="D12" s="195" t="s">
         <v>470</v>
       </c>
-      <c r="E12" s="177" t="s">
+      <c r="E12" s="198" t="s">
         <v>713</v>
       </c>
-      <c r="F12" s="177" t="s">
+      <c r="F12" s="198" t="s">
         <v>793</v>
       </c>
       <c r="G12" s="40">
@@ -5193,12 +5193,12 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A13" s="184"/>
-      <c r="B13" s="186"/>
-      <c r="C13" s="186"/>
-      <c r="D13" s="186"/>
-      <c r="E13" s="178"/>
-      <c r="F13" s="178"/>
+      <c r="A13" s="201"/>
+      <c r="B13" s="196"/>
+      <c r="C13" s="196"/>
+      <c r="D13" s="196"/>
+      <c r="E13" s="199"/>
+      <c r="F13" s="199"/>
       <c r="G13" s="40">
         <v>2</v>
       </c>
@@ -5216,12 +5216,12 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A14" s="184"/>
-      <c r="B14" s="186"/>
-      <c r="C14" s="186"/>
-      <c r="D14" s="186"/>
-      <c r="E14" s="178"/>
-      <c r="F14" s="178"/>
+      <c r="A14" s="201"/>
+      <c r="B14" s="196"/>
+      <c r="C14" s="196"/>
+      <c r="D14" s="196"/>
+      <c r="E14" s="199"/>
+      <c r="F14" s="199"/>
       <c r="G14" s="40">
         <v>3</v>
       </c>
@@ -5239,12 +5239,12 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A15" s="184"/>
-      <c r="B15" s="187"/>
-      <c r="C15" s="187"/>
-      <c r="D15" s="187"/>
-      <c r="E15" s="179"/>
-      <c r="F15" s="179"/>
+      <c r="A15" s="201"/>
+      <c r="B15" s="197"/>
+      <c r="C15" s="197"/>
+      <c r="D15" s="197"/>
+      <c r="E15" s="200"/>
+      <c r="F15" s="200"/>
       <c r="G15" s="40">
         <v>4</v>
       </c>
@@ -5255,11 +5255,11 @@
     </row>
     <row r="16" spans="1:11" ht="45.75" customHeight="1">
       <c r="A16" s="35"/>
-      <c r="B16" s="180" t="s">
+      <c r="B16" s="202" t="s">
         <v>372</v>
       </c>
-      <c r="C16" s="180"/>
-      <c r="D16" s="180"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
       <c r="E16" s="151"/>
       <c r="F16" s="151"/>
       <c r="G16" s="35"/>
@@ -5269,22 +5269,22 @@
       <c r="K16" s="36"/>
     </row>
     <row r="17" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A17" s="184" t="s">
+      <c r="A17" s="201" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="185" t="s">
+      <c r="B17" s="195" t="s">
         <v>468</v>
       </c>
-      <c r="C17" s="185" t="s">
+      <c r="C17" s="195" t="s">
         <v>471</v>
       </c>
-      <c r="D17" s="185" t="s">
+      <c r="D17" s="195" t="s">
         <v>472</v>
       </c>
-      <c r="E17" s="177" t="s">
+      <c r="E17" s="198" t="s">
         <v>794</v>
       </c>
-      <c r="F17" s="177" t="s">
+      <c r="F17" s="198" t="s">
         <v>758</v>
       </c>
       <c r="G17" s="40">
@@ -5304,12 +5304,12 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A18" s="184"/>
-      <c r="B18" s="186"/>
-      <c r="C18" s="186"/>
-      <c r="D18" s="186"/>
-      <c r="E18" s="178"/>
-      <c r="F18" s="178"/>
+      <c r="A18" s="201"/>
+      <c r="B18" s="196"/>
+      <c r="C18" s="196"/>
+      <c r="D18" s="196"/>
+      <c r="E18" s="199"/>
+      <c r="F18" s="199"/>
       <c r="G18" s="40">
         <v>2</v>
       </c>
@@ -5327,12 +5327,12 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A19" s="184"/>
-      <c r="B19" s="186"/>
-      <c r="C19" s="186"/>
-      <c r="D19" s="186"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="178"/>
+      <c r="A19" s="201"/>
+      <c r="B19" s="196"/>
+      <c r="C19" s="196"/>
+      <c r="D19" s="196"/>
+      <c r="E19" s="199"/>
+      <c r="F19" s="199"/>
       <c r="G19" s="40">
         <v>3</v>
       </c>
@@ -5350,12 +5350,12 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A20" s="184"/>
-      <c r="B20" s="187"/>
-      <c r="C20" s="187"/>
-      <c r="D20" s="187"/>
-      <c r="E20" s="179"/>
-      <c r="F20" s="179"/>
+      <c r="A20" s="201"/>
+      <c r="B20" s="197"/>
+      <c r="C20" s="197"/>
+      <c r="D20" s="197"/>
+      <c r="E20" s="200"/>
+      <c r="F20" s="200"/>
       <c r="G20" s="40">
         <v>4</v>
       </c>
@@ -5366,11 +5366,11 @@
     </row>
     <row r="21" spans="1:11" ht="45.75" customHeight="1">
       <c r="A21" s="35"/>
-      <c r="B21" s="180" t="s">
+      <c r="B21" s="202" t="s">
         <v>373</v>
       </c>
-      <c r="C21" s="180"/>
-      <c r="D21" s="180"/>
+      <c r="C21" s="202"/>
+      <c r="D21" s="202"/>
       <c r="E21" s="151"/>
       <c r="F21" s="151"/>
       <c r="G21" s="35"/>
@@ -5380,22 +5380,22 @@
       <c r="K21" s="36"/>
     </row>
     <row r="22" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A22" s="177" t="s">
+      <c r="A22" s="198" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="195" t="s">
         <v>473</v>
       </c>
-      <c r="C22" s="185" t="s">
+      <c r="C22" s="195" t="s">
         <v>474</v>
       </c>
-      <c r="D22" s="185" t="s">
+      <c r="D22" s="195" t="s">
         <v>475</v>
       </c>
-      <c r="E22" s="177" t="s">
+      <c r="E22" s="198" t="s">
         <v>795</v>
       </c>
-      <c r="F22" s="177" t="s">
+      <c r="F22" s="198" t="s">
         <v>758</v>
       </c>
       <c r="G22" s="40">
@@ -5415,12 +5415,12 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A23" s="178"/>
-      <c r="B23" s="186"/>
-      <c r="C23" s="186"/>
-      <c r="D23" s="186"/>
-      <c r="E23" s="178"/>
-      <c r="F23" s="178"/>
+      <c r="A23" s="199"/>
+      <c r="B23" s="196"/>
+      <c r="C23" s="196"/>
+      <c r="D23" s="196"/>
+      <c r="E23" s="199"/>
+      <c r="F23" s="199"/>
       <c r="G23" s="40">
         <v>2</v>
       </c>
@@ -5438,12 +5438,12 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A24" s="178"/>
-      <c r="B24" s="186"/>
-      <c r="C24" s="186"/>
-      <c r="D24" s="186"/>
-      <c r="E24" s="178"/>
-      <c r="F24" s="178"/>
+      <c r="A24" s="199"/>
+      <c r="B24" s="196"/>
+      <c r="C24" s="196"/>
+      <c r="D24" s="196"/>
+      <c r="E24" s="199"/>
+      <c r="F24" s="199"/>
       <c r="G24" s="40">
         <v>3</v>
       </c>
@@ -5461,12 +5461,12 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A25" s="178"/>
-      <c r="B25" s="186"/>
-      <c r="C25" s="186"/>
-      <c r="D25" s="186"/>
-      <c r="E25" s="178"/>
-      <c r="F25" s="178"/>
+      <c r="A25" s="199"/>
+      <c r="B25" s="196"/>
+      <c r="C25" s="196"/>
+      <c r="D25" s="196"/>
+      <c r="E25" s="199"/>
+      <c r="F25" s="199"/>
       <c r="G25" s="40">
         <v>4</v>
       </c>
@@ -5484,12 +5484,12 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A26" s="178"/>
-      <c r="B26" s="186"/>
-      <c r="C26" s="186"/>
-      <c r="D26" s="186"/>
-      <c r="E26" s="178"/>
-      <c r="F26" s="178"/>
+      <c r="A26" s="199"/>
+      <c r="B26" s="196"/>
+      <c r="C26" s="196"/>
+      <c r="D26" s="196"/>
+      <c r="E26" s="199"/>
+      <c r="F26" s="199"/>
       <c r="G26" s="40">
         <v>5</v>
       </c>
@@ -5507,12 +5507,12 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A27" s="179"/>
-      <c r="B27" s="187"/>
-      <c r="C27" s="187"/>
-      <c r="D27" s="187"/>
-      <c r="E27" s="179"/>
-      <c r="F27" s="179"/>
+      <c r="A27" s="200"/>
+      <c r="B27" s="197"/>
+      <c r="C27" s="197"/>
+      <c r="D27" s="197"/>
+      <c r="E27" s="200"/>
+      <c r="F27" s="200"/>
       <c r="G27" s="40">
         <v>6</v>
       </c>
@@ -5531,20 +5531,14 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="F22:F27"/>
+    <mergeCell ref="E22:E27"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="F17:F20"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="B3:D3"/>
@@ -5560,14 +5554,20 @@
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F22:F27"/>
-    <mergeCell ref="E22:E27"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="F17:F20"/>
+    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5590,28 +5590,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="191" t="s">
         <v>568</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="192" t="s">
         <v>569</v>
       </c>
-      <c r="C1" s="175" t="s">
+      <c r="C1" s="193" t="s">
         <v>580</v>
       </c>
-      <c r="D1" s="175" t="s">
+      <c r="D1" s="193" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="174" t="s">
+      <c r="E1" s="192" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="173"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="174"/>
+      <c r="A2" s="191"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="194"/>
+      <c r="D2" s="194"/>
+      <c r="E2" s="192"/>
     </row>
     <row r="3" spans="1:5" s="72" customFormat="1">
       <c r="A3" s="73" t="s">
@@ -5629,13 +5629,13 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="193" t="s">
+      <c r="A4" s="211" t="s">
         <v>586</v>
       </c>
-      <c r="B4" s="195">
+      <c r="B4" s="213">
         <v>45245</v>
       </c>
-      <c r="C4" s="195" t="s">
+      <c r="C4" s="213" t="s">
         <v>582</v>
       </c>
       <c r="D4" s="110"/>
@@ -5644,31 +5644,31 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="194"/>
-      <c r="B5" s="196"/>
-      <c r="C5" s="200"/>
+      <c r="A5" s="212"/>
+      <c r="B5" s="214"/>
+      <c r="C5" s="218"/>
       <c r="D5" s="111"/>
       <c r="E5" s="68" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="194"/>
-      <c r="B6" s="196"/>
-      <c r="C6" s="201"/>
+      <c r="A6" s="212"/>
+      <c r="B6" s="214"/>
+      <c r="C6" s="219"/>
       <c r="D6" s="111"/>
       <c r="E6" s="68" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="193" t="s">
+      <c r="A7" s="211" t="s">
         <v>587</v>
       </c>
-      <c r="B7" s="195">
+      <c r="B7" s="213">
         <v>45261</v>
       </c>
-      <c r="C7" s="195" t="s">
+      <c r="C7" s="213" t="s">
         <v>583</v>
       </c>
       <c r="D7" s="110"/>
@@ -5677,31 +5677,31 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="194"/>
-      <c r="B8" s="196"/>
-      <c r="C8" s="200"/>
+      <c r="A8" s="212"/>
+      <c r="B8" s="214"/>
+      <c r="C8" s="218"/>
       <c r="D8" s="111"/>
       <c r="E8" s="68" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="194"/>
-      <c r="B9" s="196"/>
-      <c r="C9" s="201"/>
+      <c r="A9" s="212"/>
+      <c r="B9" s="214"/>
+      <c r="C9" s="219"/>
       <c r="D9" s="111"/>
       <c r="E9" s="68" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="193" t="s">
+      <c r="A10" s="211" t="s">
         <v>588</v>
       </c>
-      <c r="B10" s="197">
+      <c r="B10" s="215">
         <v>45265</v>
       </c>
-      <c r="C10" s="195" t="s">
+      <c r="C10" s="213" t="s">
         <v>584</v>
       </c>
       <c r="D10" s="105"/>
@@ -5710,9 +5710,9 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="199"/>
-      <c r="B11" s="198"/>
-      <c r="C11" s="201"/>
+      <c r="A11" s="217"/>
+      <c r="B11" s="216"/>
+      <c r="C11" s="219"/>
       <c r="D11" s="109"/>
       <c r="E11" s="76" t="s">
         <v>579</v>
@@ -5821,20 +5821,20 @@
   <sheetData>
     <row r="1" spans="1:11" ht="29.25" customHeight="1">
       <c r="A1" s="19"/>
-      <c r="B1" s="208" t="s">
+      <c r="B1" s="239" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="209"/>
-      <c r="D1" s="209"/>
-      <c r="E1" s="209"/>
-      <c r="F1" s="209"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="211" t="s">
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
+      <c r="F1" s="240"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="242" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="212"/>
-      <c r="J1" s="212"/>
-      <c r="K1" s="213"/>
+      <c r="I1" s="243"/>
+      <c r="J1" s="243"/>
+      <c r="K1" s="244"/>
     </row>
     <row r="2" spans="1:11" ht="29.25" customHeight="1">
       <c r="A2" s="18" t="s">
@@ -5873,11 +5873,11 @@
     </row>
     <row r="3" spans="1:11" s="37" customFormat="1" ht="29.25" customHeight="1">
       <c r="A3" s="35"/>
-      <c r="B3" s="180" t="s">
+      <c r="B3" s="202" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
       <c r="E3" s="151"/>
       <c r="F3" s="151"/>
       <c r="G3" s="35"/>
@@ -5887,22 +5887,22 @@
       <c r="K3" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A4" s="184" t="s">
+      <c r="A4" s="201" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="184" t="s">
+      <c r="B4" s="201" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="214" t="s">
+      <c r="C4" s="231" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="215" t="s">
+      <c r="D4" s="232" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="177" t="s">
+      <c r="E4" s="198" t="s">
         <v>714</v>
       </c>
-      <c r="F4" s="177" t="s">
+      <c r="F4" s="198" t="s">
         <v>383</v>
       </c>
       <c r="G4" s="26">
@@ -5922,12 +5922,12 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A5" s="184"/>
-      <c r="B5" s="184"/>
-      <c r="C5" s="214"/>
-      <c r="D5" s="215"/>
-      <c r="E5" s="178"/>
-      <c r="F5" s="178"/>
+      <c r="A5" s="201"/>
+      <c r="B5" s="201"/>
+      <c r="C5" s="231"/>
+      <c r="D5" s="232"/>
+      <c r="E5" s="199"/>
+      <c r="F5" s="199"/>
       <c r="G5" s="26">
         <v>2</v>
       </c>
@@ -5943,12 +5943,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A6" s="184"/>
-      <c r="B6" s="184"/>
-      <c r="C6" s="214"/>
-      <c r="D6" s="215"/>
-      <c r="E6" s="178"/>
-      <c r="F6" s="178"/>
+      <c r="A6" s="201"/>
+      <c r="B6" s="201"/>
+      <c r="C6" s="231"/>
+      <c r="D6" s="232"/>
+      <c r="E6" s="199"/>
+      <c r="F6" s="199"/>
       <c r="G6" s="26">
         <v>3</v>
       </c>
@@ -5964,12 +5964,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A7" s="184"/>
-      <c r="B7" s="184"/>
-      <c r="C7" s="214"/>
-      <c r="D7" s="215"/>
-      <c r="E7" s="179"/>
-      <c r="F7" s="179"/>
+      <c r="A7" s="201"/>
+      <c r="B7" s="201"/>
+      <c r="C7" s="231"/>
+      <c r="D7" s="232"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="200"/>
       <c r="G7" s="26">
         <v>4</v>
       </c>
@@ -5988,11 +5988,11 @@
     </row>
     <row r="8" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A8" s="31"/>
-      <c r="B8" s="188" t="s">
+      <c r="B8" s="206" t="s">
         <v>330</v>
       </c>
-      <c r="C8" s="189"/>
-      <c r="D8" s="190"/>
+      <c r="C8" s="207"/>
+      <c r="D8" s="208"/>
       <c r="E8" s="132"/>
       <c r="F8" s="132"/>
       <c r="G8" s="27"/>
@@ -6002,22 +6002,22 @@
       <c r="K8" s="28"/>
     </row>
     <row r="9" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A9" s="202" t="s">
+      <c r="A9" s="220" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="220" t="s">
+      <c r="B9" s="223" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="219" t="s">
+      <c r="C9" s="227" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="219" t="s">
+      <c r="D9" s="227" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="202" t="s">
+      <c r="E9" s="220" t="s">
         <v>383</v>
       </c>
-      <c r="F9" s="202" t="s">
+      <c r="F9" s="220" t="s">
         <v>762</v>
       </c>
       <c r="G9" s="26">
@@ -6035,12 +6035,12 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A10" s="203"/>
-      <c r="B10" s="220"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="203"/>
-      <c r="F10" s="203"/>
+      <c r="A10" s="221"/>
+      <c r="B10" s="223"/>
+      <c r="C10" s="227"/>
+      <c r="D10" s="227"/>
+      <c r="E10" s="221"/>
+      <c r="F10" s="221"/>
       <c r="G10" s="26">
         <v>2</v>
       </c>
@@ -6058,12 +6058,12 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A11" s="203"/>
-      <c r="B11" s="220"/>
-      <c r="C11" s="219"/>
-      <c r="D11" s="219"/>
-      <c r="E11" s="203"/>
-      <c r="F11" s="203"/>
+      <c r="A11" s="221"/>
+      <c r="B11" s="223"/>
+      <c r="C11" s="227"/>
+      <c r="D11" s="227"/>
+      <c r="E11" s="221"/>
+      <c r="F11" s="221"/>
       <c r="G11" s="26">
         <v>3</v>
       </c>
@@ -6081,12 +6081,12 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A12" s="203"/>
-      <c r="B12" s="220"/>
-      <c r="C12" s="219"/>
-      <c r="D12" s="219"/>
-      <c r="E12" s="203"/>
-      <c r="F12" s="203"/>
+      <c r="A12" s="221"/>
+      <c r="B12" s="223"/>
+      <c r="C12" s="227"/>
+      <c r="D12" s="227"/>
+      <c r="E12" s="221"/>
+      <c r="F12" s="221"/>
       <c r="G12" s="128">
         <v>4</v>
       </c>
@@ -6098,12 +6098,12 @@
       <c r="K12" s="42"/>
     </row>
     <row r="13" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A13" s="203"/>
-      <c r="B13" s="220"/>
-      <c r="C13" s="219"/>
-      <c r="D13" s="219"/>
-      <c r="E13" s="203"/>
-      <c r="F13" s="203"/>
+      <c r="A13" s="221"/>
+      <c r="B13" s="223"/>
+      <c r="C13" s="227"/>
+      <c r="D13" s="227"/>
+      <c r="E13" s="221"/>
+      <c r="F13" s="221"/>
       <c r="G13" s="128">
         <v>5</v>
       </c>
@@ -6115,12 +6115,12 @@
       <c r="K13" s="42"/>
     </row>
     <row r="14" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A14" s="203"/>
-      <c r="B14" s="220"/>
-      <c r="C14" s="219"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="203"/>
-      <c r="F14" s="203"/>
+      <c r="A14" s="221"/>
+      <c r="B14" s="223"/>
+      <c r="C14" s="227"/>
+      <c r="D14" s="227"/>
+      <c r="E14" s="221"/>
+      <c r="F14" s="221"/>
       <c r="G14" s="128">
         <v>6</v>
       </c>
@@ -6132,12 +6132,12 @@
       <c r="K14" s="42"/>
     </row>
     <row r="15" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A15" s="204"/>
-      <c r="B15" s="220"/>
-      <c r="C15" s="219"/>
-      <c r="D15" s="219"/>
-      <c r="E15" s="204"/>
-      <c r="F15" s="204"/>
+      <c r="A15" s="222"/>
+      <c r="B15" s="223"/>
+      <c r="C15" s="227"/>
+      <c r="D15" s="227"/>
+      <c r="E15" s="222"/>
+      <c r="F15" s="222"/>
       <c r="G15" s="128">
         <v>7</v>
       </c>
@@ -6156,11 +6156,11 @@
     </row>
     <row r="16" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A16" s="32"/>
-      <c r="B16" s="216" t="s">
+      <c r="B16" s="224" t="s">
         <v>332</v>
       </c>
-      <c r="C16" s="217"/>
-      <c r="D16" s="218"/>
+      <c r="C16" s="225"/>
+      <c r="D16" s="226"/>
       <c r="E16" s="133"/>
       <c r="F16" s="133"/>
       <c r="G16" s="27"/>
@@ -6170,22 +6170,22 @@
       <c r="K16" s="28"/>
     </row>
     <row r="17" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A17" s="202" t="s">
+      <c r="A17" s="220" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="220" t="s">
+      <c r="B17" s="223" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="221" t="s">
+      <c r="C17" s="228" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="220" t="s">
+      <c r="D17" s="223" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="202" t="s">
+      <c r="E17" s="220" t="s">
         <v>383</v>
       </c>
-      <c r="F17" s="202" t="s">
+      <c r="F17" s="220" t="s">
         <v>759</v>
       </c>
       <c r="G17" s="26">
@@ -6205,12 +6205,12 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A18" s="203"/>
-      <c r="B18" s="220"/>
-      <c r="C18" s="222"/>
-      <c r="D18" s="220"/>
-      <c r="E18" s="203"/>
-      <c r="F18" s="203"/>
+      <c r="A18" s="221"/>
+      <c r="B18" s="223"/>
+      <c r="C18" s="229"/>
+      <c r="D18" s="223"/>
+      <c r="E18" s="221"/>
+      <c r="F18" s="221"/>
       <c r="G18" s="26">
         <v>2</v>
       </c>
@@ -6226,12 +6226,12 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A19" s="203"/>
-      <c r="B19" s="220"/>
-      <c r="C19" s="222"/>
-      <c r="D19" s="220"/>
-      <c r="E19" s="203"/>
-      <c r="F19" s="203"/>
+      <c r="A19" s="221"/>
+      <c r="B19" s="223"/>
+      <c r="C19" s="229"/>
+      <c r="D19" s="223"/>
+      <c r="E19" s="221"/>
+      <c r="F19" s="221"/>
       <c r="G19" s="128">
         <v>3</v>
       </c>
@@ -6243,12 +6243,12 @@
       <c r="K19" s="42"/>
     </row>
     <row r="20" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A20" s="203"/>
-      <c r="B20" s="220"/>
-      <c r="C20" s="222"/>
-      <c r="D20" s="220"/>
-      <c r="E20" s="203"/>
-      <c r="F20" s="203"/>
+      <c r="A20" s="221"/>
+      <c r="B20" s="223"/>
+      <c r="C20" s="229"/>
+      <c r="D20" s="223"/>
+      <c r="E20" s="221"/>
+      <c r="F20" s="221"/>
       <c r="G20" s="128">
         <v>4</v>
       </c>
@@ -6266,12 +6266,12 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A21" s="203"/>
-      <c r="B21" s="220"/>
-      <c r="C21" s="222"/>
-      <c r="D21" s="220"/>
-      <c r="E21" s="203"/>
-      <c r="F21" s="203"/>
+      <c r="A21" s="221"/>
+      <c r="B21" s="223"/>
+      <c r="C21" s="229"/>
+      <c r="D21" s="223"/>
+      <c r="E21" s="221"/>
+      <c r="F21" s="221"/>
       <c r="G21" s="128">
         <v>5</v>
       </c>
@@ -6289,12 +6289,12 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A22" s="204"/>
-      <c r="B22" s="220"/>
-      <c r="C22" s="223"/>
-      <c r="D22" s="220"/>
-      <c r="E22" s="204"/>
-      <c r="F22" s="204"/>
+      <c r="A22" s="222"/>
+      <c r="B22" s="223"/>
+      <c r="C22" s="230"/>
+      <c r="D22" s="223"/>
+      <c r="E22" s="222"/>
+      <c r="F22" s="222"/>
       <c r="G22" s="128">
         <v>6</v>
       </c>
@@ -6307,11 +6307,11 @@
     </row>
     <row r="23" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A23" s="27"/>
-      <c r="B23" s="188" t="s">
+      <c r="B23" s="206" t="s">
         <v>328</v>
       </c>
-      <c r="C23" s="189"/>
-      <c r="D23" s="190"/>
+      <c r="C23" s="207"/>
+      <c r="D23" s="208"/>
       <c r="E23" s="132"/>
       <c r="F23" s="132"/>
       <c r="G23" s="27"/>
@@ -6321,22 +6321,22 @@
       <c r="K23" s="28"/>
     </row>
     <row r="24" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A24" s="184" t="s">
+      <c r="A24" s="201" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="184" t="s">
+      <c r="B24" s="201" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="214" t="s">
+      <c r="C24" s="231" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="215" t="s">
+      <c r="D24" s="232" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="177" t="s">
+      <c r="E24" s="198" t="s">
         <v>383</v>
       </c>
-      <c r="F24" s="177" t="s">
+      <c r="F24" s="198" t="s">
         <v>761</v>
       </c>
       <c r="G24" s="26">
@@ -6354,12 +6354,12 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A25" s="184"/>
-      <c r="B25" s="184"/>
-      <c r="C25" s="214"/>
-      <c r="D25" s="215"/>
-      <c r="E25" s="178"/>
-      <c r="F25" s="178"/>
+      <c r="A25" s="201"/>
+      <c r="B25" s="201"/>
+      <c r="C25" s="231"/>
+      <c r="D25" s="232"/>
+      <c r="E25" s="199"/>
+      <c r="F25" s="199"/>
       <c r="G25" s="34">
         <v>2</v>
       </c>
@@ -6375,12 +6375,12 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A26" s="184"/>
-      <c r="B26" s="184"/>
-      <c r="C26" s="214"/>
-      <c r="D26" s="215"/>
-      <c r="E26" s="178"/>
-      <c r="F26" s="178"/>
+      <c r="A26" s="201"/>
+      <c r="B26" s="201"/>
+      <c r="C26" s="231"/>
+      <c r="D26" s="232"/>
+      <c r="E26" s="199"/>
+      <c r="F26" s="199"/>
       <c r="G26" s="26">
         <v>3</v>
       </c>
@@ -6396,12 +6396,12 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A27" s="184"/>
-      <c r="B27" s="184"/>
-      <c r="C27" s="214"/>
-      <c r="D27" s="215"/>
-      <c r="E27" s="179"/>
-      <c r="F27" s="179"/>
+      <c r="A27" s="201"/>
+      <c r="B27" s="201"/>
+      <c r="C27" s="231"/>
+      <c r="D27" s="232"/>
+      <c r="E27" s="200"/>
+      <c r="F27" s="200"/>
       <c r="G27" s="26">
         <v>4</v>
       </c>
@@ -6420,11 +6420,11 @@
     </row>
     <row r="28" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="188" t="s">
+      <c r="B28" s="206" t="s">
         <v>329</v>
       </c>
-      <c r="C28" s="189"/>
-      <c r="D28" s="190"/>
+      <c r="C28" s="207"/>
+      <c r="D28" s="208"/>
       <c r="E28" s="132"/>
       <c r="F28" s="132"/>
       <c r="G28" s="27"/>
@@ -6434,19 +6434,19 @@
       <c r="K28" s="28"/>
     </row>
     <row r="29" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A29" s="177" t="s">
+      <c r="A29" s="198" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="177" t="s">
+      <c r="B29" s="198" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="185" t="s">
+      <c r="C29" s="195" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="224" t="s">
+      <c r="D29" s="233" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="177" t="s">
+      <c r="E29" s="198" t="s">
         <v>716</v>
       </c>
       <c r="F29" s="134"/>
@@ -6465,11 +6465,11 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A30" s="178"/>
-      <c r="B30" s="178"/>
-      <c r="C30" s="186"/>
-      <c r="D30" s="225"/>
-      <c r="E30" s="178"/>
+      <c r="A30" s="199"/>
+      <c r="B30" s="199"/>
+      <c r="C30" s="196"/>
+      <c r="D30" s="234"/>
+      <c r="E30" s="199"/>
       <c r="F30" s="135"/>
       <c r="G30" s="26">
         <v>2</v>
@@ -6486,11 +6486,11 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A31" s="178"/>
-      <c r="B31" s="178"/>
-      <c r="C31" s="186"/>
-      <c r="D31" s="225"/>
-      <c r="E31" s="178"/>
+      <c r="A31" s="199"/>
+      <c r="B31" s="199"/>
+      <c r="C31" s="196"/>
+      <c r="D31" s="234"/>
+      <c r="E31" s="199"/>
       <c r="F31" s="135"/>
       <c r="G31" s="26">
         <v>3</v>
@@ -6509,11 +6509,11 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A32" s="179"/>
-      <c r="B32" s="179"/>
-      <c r="C32" s="187"/>
-      <c r="D32" s="226"/>
-      <c r="E32" s="179"/>
+      <c r="A32" s="200"/>
+      <c r="B32" s="200"/>
+      <c r="C32" s="197"/>
+      <c r="D32" s="235"/>
+      <c r="E32" s="200"/>
       <c r="F32" s="136"/>
       <c r="G32" s="26">
         <v>4</v>
@@ -6533,11 +6533,11 @@
     </row>
     <row r="33" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A33" s="32"/>
-      <c r="B33" s="216" t="s">
+      <c r="B33" s="224" t="s">
         <v>331</v>
       </c>
-      <c r="C33" s="217"/>
-      <c r="D33" s="218"/>
+      <c r="C33" s="225"/>
+      <c r="D33" s="226"/>
       <c r="E33" s="133"/>
       <c r="F33" s="133"/>
       <c r="G33" s="27"/>
@@ -6547,22 +6547,22 @@
       <c r="K33" s="28"/>
     </row>
     <row r="34" spans="1:11" s="61" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A34" s="202" t="s">
+      <c r="A34" s="220" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="220" t="s">
+      <c r="B34" s="223" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="220" t="s">
+      <c r="C34" s="223" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="205" t="s">
+      <c r="D34" s="236" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="202" t="s">
+      <c r="E34" s="220" t="s">
         <v>715</v>
       </c>
-      <c r="F34" s="202" t="s">
+      <c r="F34" s="220" t="s">
         <v>383</v>
       </c>
       <c r="G34" s="34">
@@ -6576,12 +6576,12 @@
       <c r="K34" s="60"/>
     </row>
     <row r="35" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A35" s="203"/>
-      <c r="B35" s="220"/>
-      <c r="C35" s="220"/>
-      <c r="D35" s="206"/>
-      <c r="E35" s="203"/>
-      <c r="F35" s="203"/>
+      <c r="A35" s="221"/>
+      <c r="B35" s="223"/>
+      <c r="C35" s="223"/>
+      <c r="D35" s="237"/>
+      <c r="E35" s="221"/>
+      <c r="F35" s="221"/>
       <c r="G35" s="26">
         <v>2</v>
       </c>
@@ -6597,12 +6597,12 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A36" s="203"/>
-      <c r="B36" s="220"/>
-      <c r="C36" s="220"/>
-      <c r="D36" s="206"/>
-      <c r="E36" s="203"/>
-      <c r="F36" s="203"/>
+      <c r="A36" s="221"/>
+      <c r="B36" s="223"/>
+      <c r="C36" s="223"/>
+      <c r="D36" s="237"/>
+      <c r="E36" s="221"/>
+      <c r="F36" s="221"/>
       <c r="G36" s="34">
         <v>3</v>
       </c>
@@ -6618,12 +6618,12 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A37" s="203"/>
-      <c r="B37" s="220"/>
-      <c r="C37" s="220"/>
-      <c r="D37" s="206"/>
-      <c r="E37" s="203"/>
-      <c r="F37" s="203"/>
+      <c r="A37" s="221"/>
+      <c r="B37" s="223"/>
+      <c r="C37" s="223"/>
+      <c r="D37" s="237"/>
+      <c r="E37" s="221"/>
+      <c r="F37" s="221"/>
       <c r="G37" s="128">
         <v>4</v>
       </c>
@@ -6641,12 +6641,12 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A38" s="204"/>
-      <c r="B38" s="220"/>
-      <c r="C38" s="220"/>
-      <c r="D38" s="207"/>
-      <c r="E38" s="204"/>
-      <c r="F38" s="204"/>
+      <c r="A38" s="222"/>
+      <c r="B38" s="223"/>
+      <c r="C38" s="223"/>
+      <c r="D38" s="238"/>
+      <c r="E38" s="222"/>
+      <c r="F38" s="222"/>
       <c r="G38" s="34">
         <v>5</v>
       </c>
@@ -6665,11 +6665,11 @@
     </row>
     <row r="39" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A39" s="32"/>
-      <c r="B39" s="216" t="s">
+      <c r="B39" s="224" t="s">
         <v>333</v>
       </c>
-      <c r="C39" s="217"/>
-      <c r="D39" s="218"/>
+      <c r="C39" s="225"/>
+      <c r="D39" s="226"/>
       <c r="E39" s="133"/>
       <c r="F39" s="133"/>
       <c r="G39" s="27"/>
@@ -6679,22 +6679,22 @@
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A40" s="202" t="s">
+      <c r="A40" s="220" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="220" t="s">
+      <c r="B40" s="223" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="219" t="s">
+      <c r="C40" s="227" t="s">
         <v>83</v>
       </c>
-      <c r="D40" s="219" t="s">
+      <c r="D40" s="227" t="s">
         <v>84</v>
       </c>
-      <c r="E40" s="202" t="s">
+      <c r="E40" s="220" t="s">
         <v>720</v>
       </c>
-      <c r="F40" s="202" t="s">
+      <c r="F40" s="220" t="s">
         <v>383</v>
       </c>
       <c r="G40" s="26">
@@ -6712,12 +6712,12 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A41" s="203"/>
-      <c r="B41" s="220"/>
-      <c r="C41" s="219"/>
-      <c r="D41" s="219"/>
-      <c r="E41" s="203"/>
-      <c r="F41" s="203"/>
+      <c r="A41" s="221"/>
+      <c r="B41" s="223"/>
+      <c r="C41" s="227"/>
+      <c r="D41" s="227"/>
+      <c r="E41" s="221"/>
+      <c r="F41" s="221"/>
       <c r="G41" s="26">
         <v>2</v>
       </c>
@@ -6733,12 +6733,12 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A42" s="203"/>
-      <c r="B42" s="220"/>
-      <c r="C42" s="219"/>
-      <c r="D42" s="219"/>
-      <c r="E42" s="203"/>
-      <c r="F42" s="203"/>
+      <c r="A42" s="221"/>
+      <c r="B42" s="223"/>
+      <c r="C42" s="227"/>
+      <c r="D42" s="227"/>
+      <c r="E42" s="221"/>
+      <c r="F42" s="221"/>
       <c r="G42" s="26">
         <v>3</v>
       </c>
@@ -6756,12 +6756,12 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A43" s="204"/>
-      <c r="B43" s="220"/>
-      <c r="C43" s="219"/>
-      <c r="D43" s="219"/>
-      <c r="E43" s="204"/>
-      <c r="F43" s="204"/>
+      <c r="A43" s="222"/>
+      <c r="B43" s="223"/>
+      <c r="C43" s="227"/>
+      <c r="D43" s="227"/>
+      <c r="E43" s="222"/>
+      <c r="F43" s="222"/>
       <c r="G43" s="26">
         <v>4</v>
       </c>
@@ -6780,11 +6780,11 @@
     </row>
     <row r="44" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A44" s="32"/>
-      <c r="B44" s="216" t="s">
+      <c r="B44" s="224" t="s">
         <v>334</v>
       </c>
-      <c r="C44" s="217"/>
-      <c r="D44" s="218"/>
+      <c r="C44" s="225"/>
+      <c r="D44" s="226"/>
       <c r="E44" s="133"/>
       <c r="F44" s="133"/>
       <c r="G44" s="27"/>
@@ -6794,22 +6794,22 @@
       <c r="K44" s="33"/>
     </row>
     <row r="45" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A45" s="202" t="s">
+      <c r="A45" s="220" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="220" t="s">
+      <c r="B45" s="223" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="219" t="s">
+      <c r="C45" s="227" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="219" t="s">
+      <c r="D45" s="227" t="s">
         <v>86</v>
       </c>
-      <c r="E45" s="202" t="s">
+      <c r="E45" s="220" t="s">
         <v>712</v>
       </c>
-      <c r="F45" s="202" t="s">
+      <c r="F45" s="220" t="s">
         <v>383</v>
       </c>
       <c r="G45" s="26">
@@ -6829,12 +6829,12 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A46" s="203"/>
-      <c r="B46" s="220"/>
-      <c r="C46" s="219"/>
-      <c r="D46" s="219"/>
-      <c r="E46" s="203"/>
-      <c r="F46" s="203"/>
+      <c r="A46" s="221"/>
+      <c r="B46" s="223"/>
+      <c r="C46" s="227"/>
+      <c r="D46" s="227"/>
+      <c r="E46" s="221"/>
+      <c r="F46" s="221"/>
       <c r="G46" s="26">
         <v>2</v>
       </c>
@@ -6852,12 +6852,12 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A47" s="203"/>
-      <c r="B47" s="220"/>
-      <c r="C47" s="219"/>
-      <c r="D47" s="219"/>
-      <c r="E47" s="203"/>
-      <c r="F47" s="203"/>
+      <c r="A47" s="221"/>
+      <c r="B47" s="223"/>
+      <c r="C47" s="227"/>
+      <c r="D47" s="227"/>
+      <c r="E47" s="221"/>
+      <c r="F47" s="221"/>
       <c r="G47" s="26">
         <v>3</v>
       </c>
@@ -6875,12 +6875,12 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A48" s="204"/>
-      <c r="B48" s="220"/>
-      <c r="C48" s="219"/>
-      <c r="D48" s="219"/>
-      <c r="E48" s="204"/>
-      <c r="F48" s="204"/>
+      <c r="A48" s="222"/>
+      <c r="B48" s="223"/>
+      <c r="C48" s="227"/>
+      <c r="D48" s="227"/>
+      <c r="E48" s="222"/>
+      <c r="F48" s="222"/>
       <c r="G48" s="26">
         <v>4</v>
       </c>
@@ -6899,11 +6899,11 @@
     </row>
     <row r="49" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A49" s="32"/>
-      <c r="B49" s="216" t="s">
+      <c r="B49" s="224" t="s">
         <v>335</v>
       </c>
-      <c r="C49" s="217"/>
-      <c r="D49" s="218"/>
+      <c r="C49" s="225"/>
+      <c r="D49" s="226"/>
       <c r="E49" s="133"/>
       <c r="F49" s="133"/>
       <c r="G49" s="27"/>
@@ -6913,22 +6913,22 @@
       <c r="K49" s="33"/>
     </row>
     <row r="50" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A50" s="202" t="s">
+      <c r="A50" s="220" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="220" t="s">
+      <c r="B50" s="223" t="s">
         <v>87</v>
       </c>
-      <c r="C50" s="219" t="s">
+      <c r="C50" s="227" t="s">
         <v>88</v>
       </c>
-      <c r="D50" s="219" t="s">
+      <c r="D50" s="227" t="s">
         <v>89</v>
       </c>
-      <c r="E50" s="202" t="s">
+      <c r="E50" s="220" t="s">
         <v>383</v>
       </c>
-      <c r="F50" s="202" t="s">
+      <c r="F50" s="220" t="s">
         <v>762</v>
       </c>
       <c r="G50" s="26">
@@ -6948,12 +6948,12 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A51" s="203"/>
-      <c r="B51" s="220"/>
-      <c r="C51" s="219"/>
-      <c r="D51" s="219"/>
-      <c r="E51" s="203"/>
-      <c r="F51" s="203"/>
+      <c r="A51" s="221"/>
+      <c r="B51" s="223"/>
+      <c r="C51" s="227"/>
+      <c r="D51" s="227"/>
+      <c r="E51" s="221"/>
+      <c r="F51" s="221"/>
       <c r="G51" s="26">
         <v>2</v>
       </c>
@@ -6969,12 +6969,12 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A52" s="203"/>
-      <c r="B52" s="220"/>
-      <c r="C52" s="219"/>
-      <c r="D52" s="219"/>
-      <c r="E52" s="203"/>
-      <c r="F52" s="203"/>
+      <c r="A52" s="221"/>
+      <c r="B52" s="223"/>
+      <c r="C52" s="227"/>
+      <c r="D52" s="227"/>
+      <c r="E52" s="221"/>
+      <c r="F52" s="221"/>
       <c r="G52" s="26">
         <v>3</v>
       </c>
@@ -6992,12 +6992,12 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A53" s="204"/>
-      <c r="B53" s="220"/>
-      <c r="C53" s="219"/>
-      <c r="D53" s="219"/>
-      <c r="E53" s="204"/>
-      <c r="F53" s="204"/>
+      <c r="A53" s="222"/>
+      <c r="B53" s="223"/>
+      <c r="C53" s="227"/>
+      <c r="D53" s="227"/>
+      <c r="E53" s="222"/>
+      <c r="F53" s="222"/>
       <c r="G53" s="26">
         <v>4</v>
       </c>
@@ -7016,11 +7016,11 @@
     </row>
     <row r="54" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A54" s="32"/>
-      <c r="B54" s="216" t="s">
+      <c r="B54" s="224" t="s">
         <v>336</v>
       </c>
-      <c r="C54" s="217"/>
-      <c r="D54" s="218"/>
+      <c r="C54" s="225"/>
+      <c r="D54" s="226"/>
       <c r="E54" s="133"/>
       <c r="F54" s="133"/>
       <c r="G54" s="27"/>
@@ -7030,22 +7030,22 @@
       <c r="K54" s="33"/>
     </row>
     <row r="55" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A55" s="202" t="s">
+      <c r="A55" s="220" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="220" t="s">
+      <c r="B55" s="223" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="219" t="s">
+      <c r="C55" s="227" t="s">
         <v>91</v>
       </c>
-      <c r="D55" s="219" t="s">
+      <c r="D55" s="227" t="s">
         <v>92</v>
       </c>
-      <c r="E55" s="202" t="s">
+      <c r="E55" s="220" t="s">
         <v>383</v>
       </c>
-      <c r="F55" s="202" t="s">
+      <c r="F55" s="220" t="s">
         <v>759</v>
       </c>
       <c r="G55" s="26">
@@ -7065,12 +7065,12 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A56" s="203"/>
-      <c r="B56" s="220"/>
-      <c r="C56" s="219"/>
-      <c r="D56" s="219"/>
-      <c r="E56" s="203"/>
-      <c r="F56" s="203"/>
+      <c r="A56" s="221"/>
+      <c r="B56" s="223"/>
+      <c r="C56" s="227"/>
+      <c r="D56" s="227"/>
+      <c r="E56" s="221"/>
+      <c r="F56" s="221"/>
       <c r="G56" s="26">
         <v>2</v>
       </c>
@@ -7088,12 +7088,12 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A57" s="203"/>
-      <c r="B57" s="220"/>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="203"/>
-      <c r="F57" s="203"/>
+      <c r="A57" s="221"/>
+      <c r="B57" s="223"/>
+      <c r="C57" s="227"/>
+      <c r="D57" s="227"/>
+      <c r="E57" s="221"/>
+      <c r="F57" s="221"/>
       <c r="G57" s="26">
         <v>3</v>
       </c>
@@ -7111,12 +7111,12 @@
       </c>
     </row>
     <row r="58" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A58" s="204"/>
-      <c r="B58" s="220"/>
-      <c r="C58" s="219"/>
-      <c r="D58" s="219"/>
-      <c r="E58" s="204"/>
-      <c r="F58" s="204"/>
+      <c r="A58" s="222"/>
+      <c r="B58" s="223"/>
+      <c r="C58" s="227"/>
+      <c r="D58" s="227"/>
+      <c r="E58" s="222"/>
+      <c r="F58" s="222"/>
       <c r="G58" s="26">
         <v>4</v>
       </c>
@@ -7135,11 +7135,11 @@
     </row>
     <row r="59" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A59" s="32"/>
-      <c r="B59" s="216" t="s">
+      <c r="B59" s="224" t="s">
         <v>337</v>
       </c>
-      <c r="C59" s="217"/>
-      <c r="D59" s="218"/>
+      <c r="C59" s="225"/>
+      <c r="D59" s="226"/>
       <c r="E59" s="133"/>
       <c r="F59" s="133"/>
       <c r="G59" s="27"/>
@@ -7149,22 +7149,22 @@
       <c r="K59" s="33"/>
     </row>
     <row r="60" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A60" s="202" t="s">
+      <c r="A60" s="220" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="220" t="s">
+      <c r="B60" s="223" t="s">
         <v>90</v>
       </c>
-      <c r="C60" s="219" t="s">
+      <c r="C60" s="227" t="s">
         <v>93</v>
       </c>
-      <c r="D60" s="219" t="s">
+      <c r="D60" s="227" t="s">
         <v>94</v>
       </c>
-      <c r="E60" s="202" t="s">
+      <c r="E60" s="220" t="s">
         <v>383</v>
       </c>
-      <c r="F60" s="202" t="s">
+      <c r="F60" s="220" t="s">
         <v>721</v>
       </c>
       <c r="G60" s="26">
@@ -7182,12 +7182,12 @@
       </c>
     </row>
     <row r="61" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A61" s="203"/>
-      <c r="B61" s="220"/>
-      <c r="C61" s="219"/>
-      <c r="D61" s="219"/>
-      <c r="E61" s="203"/>
-      <c r="F61" s="203"/>
+      <c r="A61" s="221"/>
+      <c r="B61" s="223"/>
+      <c r="C61" s="227"/>
+      <c r="D61" s="227"/>
+      <c r="E61" s="221"/>
+      <c r="F61" s="221"/>
       <c r="G61" s="26">
         <v>2</v>
       </c>
@@ -7205,12 +7205,12 @@
       </c>
     </row>
     <row r="62" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A62" s="203"/>
-      <c r="B62" s="220"/>
-      <c r="C62" s="219"/>
-      <c r="D62" s="219"/>
-      <c r="E62" s="203"/>
-      <c r="F62" s="203"/>
+      <c r="A62" s="221"/>
+      <c r="B62" s="223"/>
+      <c r="C62" s="227"/>
+      <c r="D62" s="227"/>
+      <c r="E62" s="221"/>
+      <c r="F62" s="221"/>
       <c r="G62" s="26">
         <v>3</v>
       </c>
@@ -7228,12 +7228,12 @@
       </c>
     </row>
     <row r="63" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A63" s="204"/>
-      <c r="B63" s="220"/>
-      <c r="C63" s="219"/>
-      <c r="D63" s="219"/>
-      <c r="E63" s="204"/>
-      <c r="F63" s="204"/>
+      <c r="A63" s="222"/>
+      <c r="B63" s="223"/>
+      <c r="C63" s="227"/>
+      <c r="D63" s="227"/>
+      <c r="E63" s="222"/>
+      <c r="F63" s="222"/>
       <c r="G63" s="26">
         <v>4</v>
       </c>
@@ -7252,11 +7252,11 @@
     </row>
     <row r="64" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A64" s="32"/>
-      <c r="B64" s="216" t="s">
+      <c r="B64" s="224" t="s">
         <v>338</v>
       </c>
-      <c r="C64" s="217"/>
-      <c r="D64" s="218"/>
+      <c r="C64" s="225"/>
+      <c r="D64" s="226"/>
       <c r="E64" s="133"/>
       <c r="F64" s="133"/>
       <c r="G64" s="27"/>
@@ -7266,22 +7266,22 @@
       <c r="K64" s="33"/>
     </row>
     <row r="65" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A65" s="202" t="s">
+      <c r="A65" s="220" t="s">
         <v>67</v>
       </c>
-      <c r="B65" s="220" t="s">
+      <c r="B65" s="223" t="s">
         <v>95</v>
       </c>
-      <c r="C65" s="219" t="s">
+      <c r="C65" s="227" t="s">
         <v>96</v>
       </c>
-      <c r="D65" s="219" t="s">
+      <c r="D65" s="227" t="s">
         <v>97</v>
       </c>
-      <c r="E65" s="202" t="s">
+      <c r="E65" s="220" t="s">
         <v>383</v>
       </c>
-      <c r="F65" s="202" t="s">
+      <c r="F65" s="220" t="s">
         <v>760</v>
       </c>
       <c r="G65" s="26">
@@ -7301,12 +7301,12 @@
       </c>
     </row>
     <row r="66" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A66" s="203"/>
-      <c r="B66" s="220"/>
-      <c r="C66" s="219"/>
-      <c r="D66" s="219"/>
-      <c r="E66" s="203"/>
-      <c r="F66" s="203"/>
+      <c r="A66" s="221"/>
+      <c r="B66" s="223"/>
+      <c r="C66" s="227"/>
+      <c r="D66" s="227"/>
+      <c r="E66" s="221"/>
+      <c r="F66" s="221"/>
       <c r="G66" s="26">
         <v>2</v>
       </c>
@@ -7324,12 +7324,12 @@
       </c>
     </row>
     <row r="67" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A67" s="203"/>
-      <c r="B67" s="220"/>
-      <c r="C67" s="219"/>
-      <c r="D67" s="219"/>
-      <c r="E67" s="203"/>
-      <c r="F67" s="203"/>
+      <c r="A67" s="221"/>
+      <c r="B67" s="223"/>
+      <c r="C67" s="227"/>
+      <c r="D67" s="227"/>
+      <c r="E67" s="221"/>
+      <c r="F67" s="221"/>
       <c r="G67" s="26">
         <v>3</v>
       </c>
@@ -7347,12 +7347,12 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A68" s="204"/>
-      <c r="B68" s="220"/>
-      <c r="C68" s="219"/>
-      <c r="D68" s="219"/>
-      <c r="E68" s="204"/>
-      <c r="F68" s="204"/>
+      <c r="A68" s="222"/>
+      <c r="B68" s="223"/>
+      <c r="C68" s="227"/>
+      <c r="D68" s="227"/>
+      <c r="E68" s="222"/>
+      <c r="F68" s="222"/>
       <c r="G68" s="26">
         <v>4</v>
       </c>
@@ -7371,11 +7371,11 @@
     </row>
     <row r="69" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A69" s="32"/>
-      <c r="B69" s="216" t="s">
+      <c r="B69" s="224" t="s">
         <v>339</v>
       </c>
-      <c r="C69" s="217"/>
-      <c r="D69" s="218"/>
+      <c r="C69" s="225"/>
+      <c r="D69" s="226"/>
       <c r="E69" s="133"/>
       <c r="F69" s="133"/>
       <c r="G69" s="27"/>
@@ -7385,22 +7385,22 @@
       <c r="K69" s="33"/>
     </row>
     <row r="70" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A70" s="202" t="s">
+      <c r="A70" s="220" t="s">
         <v>98</v>
       </c>
-      <c r="B70" s="220" t="s">
+      <c r="B70" s="223" t="s">
         <v>99</v>
       </c>
-      <c r="C70" s="219" t="s">
+      <c r="C70" s="227" t="s">
         <v>100</v>
       </c>
-      <c r="D70" s="219" t="s">
+      <c r="D70" s="227" t="s">
         <v>101</v>
       </c>
-      <c r="E70" s="202" t="s">
+      <c r="E70" s="220" t="s">
         <v>383</v>
       </c>
-      <c r="F70" s="202" t="s">
+      <c r="F70" s="220" t="s">
         <v>759</v>
       </c>
       <c r="G70" s="26">
@@ -7420,12 +7420,12 @@
       </c>
     </row>
     <row r="71" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A71" s="203"/>
-      <c r="B71" s="220"/>
-      <c r="C71" s="219"/>
-      <c r="D71" s="219"/>
-      <c r="E71" s="203"/>
-      <c r="F71" s="203"/>
+      <c r="A71" s="221"/>
+      <c r="B71" s="223"/>
+      <c r="C71" s="227"/>
+      <c r="D71" s="227"/>
+      <c r="E71" s="221"/>
+      <c r="F71" s="221"/>
       <c r="G71" s="26">
         <v>2</v>
       </c>
@@ -7441,12 +7441,12 @@
       </c>
     </row>
     <row r="72" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A72" s="203"/>
-      <c r="B72" s="220"/>
-      <c r="C72" s="219"/>
-      <c r="D72" s="219"/>
-      <c r="E72" s="203"/>
-      <c r="F72" s="203"/>
+      <c r="A72" s="221"/>
+      <c r="B72" s="223"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="E72" s="221"/>
+      <c r="F72" s="221"/>
       <c r="G72" s="26">
         <v>3</v>
       </c>
@@ -7462,12 +7462,12 @@
       </c>
     </row>
     <row r="73" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A73" s="204"/>
-      <c r="B73" s="220"/>
-      <c r="C73" s="219"/>
-      <c r="D73" s="219"/>
-      <c r="E73" s="204"/>
-      <c r="F73" s="204"/>
+      <c r="A73" s="222"/>
+      <c r="B73" s="223"/>
+      <c r="C73" s="227"/>
+      <c r="D73" s="227"/>
+      <c r="E73" s="222"/>
+      <c r="F73" s="222"/>
       <c r="G73" s="26">
         <v>4</v>
       </c>
@@ -7486,11 +7486,11 @@
     </row>
     <row r="74" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A74" s="32"/>
-      <c r="B74" s="216" t="s">
+      <c r="B74" s="224" t="s">
         <v>340</v>
       </c>
-      <c r="C74" s="217"/>
-      <c r="D74" s="218"/>
+      <c r="C74" s="225"/>
+      <c r="D74" s="226"/>
       <c r="E74" s="133"/>
       <c r="F74" s="133"/>
       <c r="G74" s="27"/>
@@ -7500,22 +7500,22 @@
       <c r="K74" s="33"/>
     </row>
     <row r="75" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A75" s="202" t="s">
+      <c r="A75" s="220" t="s">
         <v>102</v>
       </c>
-      <c r="B75" s="220" t="s">
+      <c r="B75" s="223" t="s">
         <v>103</v>
       </c>
-      <c r="C75" s="219" t="s">
+      <c r="C75" s="227" t="s">
         <v>104</v>
       </c>
-      <c r="D75" s="219" t="s">
+      <c r="D75" s="227" t="s">
         <v>105</v>
       </c>
-      <c r="E75" s="202" t="s">
+      <c r="E75" s="220" t="s">
         <v>383</v>
       </c>
-      <c r="F75" s="202" t="s">
+      <c r="F75" s="220" t="s">
         <v>758</v>
       </c>
       <c r="G75" s="26">
@@ -7535,12 +7535,12 @@
       </c>
     </row>
     <row r="76" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A76" s="203"/>
-      <c r="B76" s="220"/>
-      <c r="C76" s="219"/>
-      <c r="D76" s="219"/>
-      <c r="E76" s="203"/>
-      <c r="F76" s="203"/>
+      <c r="A76" s="221"/>
+      <c r="B76" s="223"/>
+      <c r="C76" s="227"/>
+      <c r="D76" s="227"/>
+      <c r="E76" s="221"/>
+      <c r="F76" s="221"/>
       <c r="G76" s="26">
         <v>2</v>
       </c>
@@ -7558,12 +7558,12 @@
       </c>
     </row>
     <row r="77" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A77" s="203"/>
-      <c r="B77" s="220"/>
-      <c r="C77" s="219"/>
-      <c r="D77" s="219"/>
-      <c r="E77" s="203"/>
-      <c r="F77" s="203"/>
+      <c r="A77" s="221"/>
+      <c r="B77" s="223"/>
+      <c r="C77" s="227"/>
+      <c r="D77" s="227"/>
+      <c r="E77" s="221"/>
+      <c r="F77" s="221"/>
       <c r="G77" s="26">
         <v>3</v>
       </c>
@@ -7581,12 +7581,12 @@
       </c>
     </row>
     <row r="78" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A78" s="204"/>
-      <c r="B78" s="220"/>
-      <c r="C78" s="219"/>
-      <c r="D78" s="219"/>
-      <c r="E78" s="204"/>
-      <c r="F78" s="204"/>
+      <c r="A78" s="222"/>
+      <c r="B78" s="223"/>
+      <c r="C78" s="227"/>
+      <c r="D78" s="227"/>
+      <c r="E78" s="222"/>
+      <c r="F78" s="222"/>
       <c r="G78" s="26">
         <v>4</v>
       </c>
@@ -7605,11 +7605,11 @@
     </row>
     <row r="79" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A79" s="32"/>
-      <c r="B79" s="216" t="s">
+      <c r="B79" s="224" t="s">
         <v>341</v>
       </c>
-      <c r="C79" s="217"/>
-      <c r="D79" s="218"/>
+      <c r="C79" s="225"/>
+      <c r="D79" s="226"/>
       <c r="E79" s="133"/>
       <c r="F79" s="133"/>
       <c r="G79" s="27"/>
@@ -7619,22 +7619,22 @@
       <c r="K79" s="33"/>
     </row>
     <row r="80" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A80" s="202" t="s">
+      <c r="A80" s="220" t="s">
         <v>106</v>
       </c>
-      <c r="B80" s="220" t="s">
+      <c r="B80" s="223" t="s">
         <v>68</v>
       </c>
-      <c r="C80" s="219" t="s">
+      <c r="C80" s="227" t="s">
         <v>107</v>
       </c>
-      <c r="D80" s="219" t="s">
+      <c r="D80" s="227" t="s">
         <v>108</v>
       </c>
-      <c r="E80" s="202" t="s">
+      <c r="E80" s="220" t="s">
         <v>383</v>
       </c>
-      <c r="F80" s="202" t="s">
+      <c r="F80" s="220" t="s">
         <v>383</v>
       </c>
       <c r="G80" s="26">
@@ -7654,12 +7654,12 @@
       </c>
     </row>
     <row r="81" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A81" s="203"/>
-      <c r="B81" s="220"/>
-      <c r="C81" s="219"/>
-      <c r="D81" s="219"/>
-      <c r="E81" s="203"/>
-      <c r="F81" s="203"/>
+      <c r="A81" s="221"/>
+      <c r="B81" s="223"/>
+      <c r="C81" s="227"/>
+      <c r="D81" s="227"/>
+      <c r="E81" s="221"/>
+      <c r="F81" s="221"/>
       <c r="G81" s="26">
         <v>2</v>
       </c>
@@ -7677,12 +7677,12 @@
       </c>
     </row>
     <row r="82" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A82" s="203"/>
-      <c r="B82" s="220"/>
-      <c r="C82" s="219"/>
-      <c r="D82" s="219"/>
-      <c r="E82" s="203"/>
-      <c r="F82" s="203"/>
+      <c r="A82" s="221"/>
+      <c r="B82" s="223"/>
+      <c r="C82" s="227"/>
+      <c r="D82" s="227"/>
+      <c r="E82" s="221"/>
+      <c r="F82" s="221"/>
       <c r="G82" s="26">
         <v>3</v>
       </c>
@@ -7700,12 +7700,12 @@
       </c>
     </row>
     <row r="83" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A83" s="204"/>
-      <c r="B83" s="220"/>
-      <c r="C83" s="219"/>
-      <c r="D83" s="219"/>
-      <c r="E83" s="204"/>
-      <c r="F83" s="204"/>
+      <c r="A83" s="222"/>
+      <c r="B83" s="223"/>
+      <c r="C83" s="227"/>
+      <c r="D83" s="227"/>
+      <c r="E83" s="222"/>
+      <c r="F83" s="222"/>
       <c r="G83" s="26">
         <v>4</v>
       </c>
@@ -7724,11 +7724,11 @@
     </row>
     <row r="84" spans="1:11" s="29" customFormat="1" ht="29.25" customHeight="1">
       <c r="A84" s="32"/>
-      <c r="B84" s="216" t="s">
+      <c r="B84" s="224" t="s">
         <v>342</v>
       </c>
-      <c r="C84" s="217"/>
-      <c r="D84" s="218"/>
+      <c r="C84" s="225"/>
+      <c r="D84" s="226"/>
       <c r="E84" s="133"/>
       <c r="F84" s="133"/>
       <c r="G84" s="27"/>
@@ -7738,22 +7738,22 @@
       <c r="K84" s="33"/>
     </row>
     <row r="85" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A85" s="202" t="s">
+      <c r="A85" s="220" t="s">
         <v>109</v>
       </c>
-      <c r="B85" s="220" t="s">
+      <c r="B85" s="223" t="s">
         <v>95</v>
       </c>
-      <c r="C85" s="219" t="s">
+      <c r="C85" s="227" t="s">
         <v>110</v>
       </c>
-      <c r="D85" s="219" t="s">
+      <c r="D85" s="227" t="s">
         <v>111</v>
       </c>
-      <c r="E85" s="202" t="s">
+      <c r="E85" s="220" t="s">
         <v>383</v>
       </c>
-      <c r="F85" s="202" t="s">
+      <c r="F85" s="220" t="s">
         <v>760</v>
       </c>
       <c r="G85" s="26">
@@ -7773,12 +7773,12 @@
       </c>
     </row>
     <row r="86" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A86" s="203"/>
-      <c r="B86" s="220"/>
-      <c r="C86" s="219"/>
-      <c r="D86" s="219"/>
-      <c r="E86" s="203"/>
-      <c r="F86" s="203"/>
+      <c r="A86" s="221"/>
+      <c r="B86" s="223"/>
+      <c r="C86" s="227"/>
+      <c r="D86" s="227"/>
+      <c r="E86" s="221"/>
+      <c r="F86" s="221"/>
       <c r="G86" s="26">
         <v>2</v>
       </c>
@@ -7796,12 +7796,12 @@
       </c>
     </row>
     <row r="87" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A87" s="203"/>
-      <c r="B87" s="220"/>
-      <c r="C87" s="219"/>
-      <c r="D87" s="219"/>
-      <c r="E87" s="203"/>
-      <c r="F87" s="203"/>
+      <c r="A87" s="221"/>
+      <c r="B87" s="223"/>
+      <c r="C87" s="227"/>
+      <c r="D87" s="227"/>
+      <c r="E87" s="221"/>
+      <c r="F87" s="221"/>
       <c r="G87" s="26">
         <v>3</v>
       </c>
@@ -7819,12 +7819,12 @@
       </c>
     </row>
     <row r="88" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A88" s="204"/>
-      <c r="B88" s="220"/>
-      <c r="C88" s="219"/>
-      <c r="D88" s="219"/>
-      <c r="E88" s="204"/>
-      <c r="F88" s="204"/>
+      <c r="A88" s="222"/>
+      <c r="B88" s="223"/>
+      <c r="C88" s="227"/>
+      <c r="D88" s="227"/>
+      <c r="E88" s="222"/>
+      <c r="F88" s="222"/>
       <c r="G88" s="26">
         <v>4</v>
       </c>
@@ -7843,49 +7843,52 @@
     </row>
   </sheetData>
   <mergeCells count="113">
-    <mergeCell ref="A85:A88"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B85:B88"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="D85:D88"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="C85:C88"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="C75:C78"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C65:C68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="D65:D68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="C45:C48"/>
-    <mergeCell ref="D50:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="D55:D58"/>
-    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="F75:F78"/>
+    <mergeCell ref="F85:F88"/>
+    <mergeCell ref="E85:E88"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="F80:F83"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="F50:F53"/>
+    <mergeCell ref="E50:E53"/>
+    <mergeCell ref="F55:F58"/>
+    <mergeCell ref="F60:F63"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="F45:F48"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E34:E38"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="F9:F15"/>
+    <mergeCell ref="E9:E15"/>
+    <mergeCell ref="E17:E22"/>
+    <mergeCell ref="F17:F22"/>
+    <mergeCell ref="D34:D38"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="D9:D15"/>
+    <mergeCell ref="C9:C15"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="E4:E7"/>
     <mergeCell ref="A40:A43"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="A17:A22"/>
@@ -7910,52 +7913,49 @@
     <mergeCell ref="D40:D43"/>
     <mergeCell ref="C40:C43"/>
     <mergeCell ref="B39:D39"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="F9:F15"/>
-    <mergeCell ref="E9:E15"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="F17:F22"/>
-    <mergeCell ref="D34:D38"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="D9:D15"/>
-    <mergeCell ref="C9:C15"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="F50:F53"/>
-    <mergeCell ref="E50:E53"/>
-    <mergeCell ref="F55:F58"/>
-    <mergeCell ref="F60:F63"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="F45:F48"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="E34:E38"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="F34:F38"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="F75:F78"/>
-    <mergeCell ref="F85:F88"/>
-    <mergeCell ref="E85:E88"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="F80:F83"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="D50:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="D55:D58"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="C75:C78"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="D65:D68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="A85:A88"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B85:B88"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="D85:D88"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="C85:C88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7978,28 +7978,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="191" t="s">
         <v>568</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="192" t="s">
         <v>569</v>
       </c>
-      <c r="C1" s="175" t="s">
+      <c r="C1" s="193" t="s">
         <v>580</v>
       </c>
       <c r="D1" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="174" t="s">
+      <c r="E1" s="192" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="173"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="176"/>
+      <c r="A2" s="191"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="194"/>
       <c r="D2" s="108"/>
-      <c r="E2" s="174"/>
+      <c r="E2" s="192"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="38" t="s">
@@ -8468,13 +8468,13 @@
       <c r="C8" s="52" t="s">
         <v>804</v>
       </c>
-      <c r="D8" s="229" t="s">
+      <c r="D8" s="173" t="s">
         <v>805</v>
       </c>
       <c r="E8" s="171" t="s">
         <v>383</v>
       </c>
-      <c r="F8" s="230" t="s">
+      <c r="F8" s="174" t="s">
         <v>383</v>
       </c>
       <c r="G8" s="51" t="s">
@@ -8879,26 +8879,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="191" t="s">
         <v>568</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="192" t="s">
         <v>569</v>
       </c>
-      <c r="C1" s="175" t="s">
+      <c r="C1" s="193" t="s">
         <v>604</v>
       </c>
       <c r="D1" s="107"/>
-      <c r="E1" s="174" t="s">
+      <c r="E1" s="192" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="173"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="176"/>
+      <c r="A2" s="191"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="194"/>
       <c r="D2" s="108"/>
-      <c r="E2" s="174"/>
+      <c r="E2" s="192"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="38" t="s">
@@ -9036,7 +9036,7 @@
       <c r="A15" s="137" t="s">
         <v>817</v>
       </c>
-      <c r="B15" s="232">
+      <c r="B15" s="176">
         <v>45278</v>
       </c>
       <c r="C15" s="92" t="s">
@@ -9059,7 +9059,7 @@
     <row r="17" spans="1:5">
       <c r="A17" s="139"/>
       <c r="B17" s="139"/>
-      <c r="C17" s="231"/>
+      <c r="C17" s="175"/>
       <c r="D17" s="139"/>
       <c r="E17" s="76" t="s">
         <v>815</v>
@@ -9080,8 +9080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E916DD94-D1B0-4F5A-A52B-CD3DDE50A874}">
   <dimension ref="A1:AE72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="AC29" sqref="AC29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25.5" customHeight="1"/>
@@ -9106,40 +9106,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="25.5" customHeight="1">
-      <c r="G1" s="227" t="s">
+      <c r="G1" s="245" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="228"/>
-      <c r="J1" s="227" t="s">
+      <c r="H1" s="246"/>
+      <c r="J1" s="245" t="s">
         <v>346</v>
       </c>
-      <c r="K1" s="228"/>
-      <c r="M1" s="227" t="s">
+      <c r="K1" s="246"/>
+      <c r="M1" s="245" t="s">
         <v>347</v>
       </c>
-      <c r="N1" s="228"/>
-      <c r="P1" s="227" t="s">
+      <c r="N1" s="246"/>
+      <c r="P1" s="245" t="s">
         <v>348</v>
       </c>
-      <c r="Q1" s="228"/>
-      <c r="S1" s="227" t="s">
+      <c r="Q1" s="246"/>
+      <c r="S1" s="245" t="s">
         <v>349</v>
       </c>
-      <c r="T1" s="228"/>
-      <c r="V1" s="227" t="s">
+      <c r="T1" s="246"/>
+      <c r="V1" s="245" t="s">
         <v>350</v>
       </c>
-      <c r="W1" s="228"/>
-      <c r="Y1" s="227" t="s">
+      <c r="W1" s="246"/>
+      <c r="Y1" s="245" t="s">
         <v>351</v>
       </c>
-      <c r="Z1" s="228"/>
+      <c r="Z1" s="246"/>
     </row>
     <row r="2" spans="1:31" s="17" customFormat="1" ht="33.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="246" t="s">
+      <c r="B2" s="190" t="s">
         <v>826</v>
       </c>
       <c r="C2" s="47" t="s">
@@ -9482,36 +9482,36 @@
       </c>
       <c r="AE6" s="62"/>
     </row>
-    <row r="7" spans="1:31" s="242" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A7" s="234"/>
-      <c r="B7" s="243"/>
-      <c r="C7" s="244"/>
-      <c r="D7" s="237"/>
-      <c r="E7" s="238"/>
-      <c r="F7" s="234"/>
-      <c r="G7" s="241"/>
-      <c r="H7" s="241"/>
-      <c r="I7" s="241"/>
-      <c r="J7" s="241"/>
-      <c r="K7" s="241"/>
-      <c r="L7" s="241"/>
-      <c r="M7" s="241"/>
-      <c r="N7" s="241"/>
-      <c r="O7" s="241"/>
-      <c r="P7" s="241"/>
-      <c r="Q7" s="241"/>
-      <c r="R7" s="241"/>
-      <c r="S7" s="241"/>
-      <c r="T7" s="241"/>
-      <c r="U7" s="241"/>
-      <c r="V7" s="241"/>
-      <c r="W7" s="241"/>
-      <c r="X7" s="241"/>
-      <c r="Y7" s="241"/>
-      <c r="Z7" s="241"/>
-      <c r="AA7" s="241"/>
-      <c r="AB7" s="241"/>
-      <c r="AE7" s="245"/>
+    <row r="7" spans="1:31" s="186" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A7" s="178"/>
+      <c r="B7" s="187"/>
+      <c r="C7" s="188"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="182"/>
+      <c r="F7" s="178"/>
+      <c r="G7" s="185"/>
+      <c r="H7" s="185"/>
+      <c r="I7" s="185"/>
+      <c r="J7" s="185"/>
+      <c r="K7" s="185"/>
+      <c r="L7" s="185"/>
+      <c r="M7" s="185"/>
+      <c r="N7" s="185"/>
+      <c r="O7" s="185"/>
+      <c r="P7" s="185"/>
+      <c r="Q7" s="185"/>
+      <c r="R7" s="185"/>
+      <c r="S7" s="185"/>
+      <c r="T7" s="185"/>
+      <c r="U7" s="185"/>
+      <c r="V7" s="185"/>
+      <c r="W7" s="185"/>
+      <c r="X7" s="185"/>
+      <c r="Y7" s="185"/>
+      <c r="Z7" s="185"/>
+      <c r="AA7" s="185"/>
+      <c r="AB7" s="185"/>
+      <c r="AE7" s="189"/>
     </row>
     <row r="8" spans="1:31" ht="25.5" customHeight="1">
       <c r="A8" s="2" t="s">
@@ -9662,11 +9662,11 @@
       <c r="AB11" s="16"/>
     </row>
     <row r="12" spans="1:31" ht="10.5" customHeight="1">
-      <c r="A12" s="234"/>
-      <c r="B12" s="243"/>
-      <c r="C12" s="244"/>
-      <c r="D12" s="237"/>
-      <c r="E12" s="238"/>
+      <c r="A12" s="178"/>
+      <c r="B12" s="187"/>
+      <c r="C12" s="188"/>
+      <c r="D12" s="181"/>
+      <c r="E12" s="182"/>
       <c r="F12" s="2"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -9948,11 +9948,11 @@
       </c>
     </row>
     <row r="17" spans="1:28" ht="10.5" customHeight="1">
-      <c r="A17" s="234"/>
-      <c r="B17" s="243"/>
-      <c r="C17" s="244"/>
-      <c r="D17" s="237"/>
-      <c r="E17" s="238"/>
+      <c r="A17" s="178"/>
+      <c r="B17" s="187"/>
+      <c r="C17" s="188"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
       <c r="F17" s="2"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
@@ -10414,11 +10414,11 @@
       </c>
     </row>
     <row r="26" spans="1:28" ht="10.5" customHeight="1">
-      <c r="A26" s="239"/>
-      <c r="B26" s="235"/>
-      <c r="C26" s="236"/>
-      <c r="D26" s="237"/>
-      <c r="E26" s="238"/>
+      <c r="A26" s="183"/>
+      <c r="B26" s="179"/>
+      <c r="C26" s="180"/>
+      <c r="D26" s="181"/>
+      <c r="E26" s="182"/>
       <c r="F26" s="4"/>
       <c r="G26" s="38"/>
       <c r="H26" s="14"/>
@@ -10447,7 +10447,7 @@
       <c r="A27" s="2" t="s">
         <v>818</v>
       </c>
-      <c r="B27" s="233" t="s">
+      <c r="B27" s="177" t="s">
         <v>804</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -10456,7 +10456,9 @@
       <c r="D27" s="52" t="s">
         <v>385</v>
       </c>
-      <c r="E27" s="10"/>
+      <c r="E27" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="38"/>
       <c r="H27" s="14"/>
@@ -10490,7 +10492,9 @@
       <c r="D28" s="52" t="s">
         <v>385</v>
       </c>
-      <c r="E28" s="10"/>
+      <c r="E28" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="38"/>
       <c r="H28" s="14"/>
@@ -10524,7 +10528,9 @@
       <c r="D29" s="52" t="s">
         <v>385</v>
       </c>
-      <c r="E29" s="10"/>
+      <c r="E29" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="38"/>
       <c r="H29" s="14"/>
@@ -10558,7 +10564,9 @@
       <c r="D30" s="52" t="s">
         <v>385</v>
       </c>
-      <c r="E30" s="10"/>
+      <c r="E30" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="38"/>
       <c r="H30" s="14"/>
@@ -10592,7 +10600,9 @@
       <c r="D31" s="52" t="s">
         <v>385</v>
       </c>
-      <c r="E31" s="10"/>
+      <c r="E31" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="38"/>
       <c r="H31" s="14"/>
@@ -10626,7 +10636,9 @@
       <c r="D32" s="52" t="s">
         <v>385</v>
       </c>
-      <c r="E32" s="10"/>
+      <c r="E32" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="38"/>
       <c r="H32" s="14"/>
@@ -10660,7 +10672,9 @@
       <c r="D33" s="52" t="s">
         <v>385</v>
       </c>
-      <c r="E33" s="10"/>
+      <c r="E33" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="38"/>
       <c r="H33" s="14"/>
@@ -10685,35 +10699,35 @@
       <c r="AA33" s="16"/>
       <c r="AB33" s="16"/>
     </row>
-    <row r="34" spans="1:28" s="242" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A34" s="234"/>
-      <c r="B34" s="235"/>
-      <c r="C34" s="236"/>
-      <c r="D34" s="237"/>
-      <c r="E34" s="238"/>
-      <c r="F34" s="239"/>
-      <c r="G34" s="240"/>
-      <c r="H34" s="241"/>
-      <c r="I34" s="241"/>
-      <c r="J34" s="240"/>
-      <c r="K34" s="240"/>
-      <c r="L34" s="241"/>
-      <c r="M34" s="240"/>
-      <c r="N34" s="240"/>
-      <c r="O34" s="241"/>
-      <c r="P34" s="240"/>
-      <c r="Q34" s="240"/>
-      <c r="R34" s="241"/>
-      <c r="S34" s="240"/>
-      <c r="T34" s="240"/>
-      <c r="U34" s="241"/>
-      <c r="V34" s="240"/>
-      <c r="W34" s="240"/>
-      <c r="X34" s="241"/>
-      <c r="Y34" s="240"/>
-      <c r="Z34" s="240"/>
-      <c r="AA34" s="241"/>
-      <c r="AB34" s="241"/>
+    <row r="34" spans="1:28" s="186" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A34" s="178"/>
+      <c r="B34" s="179"/>
+      <c r="C34" s="180"/>
+      <c r="D34" s="181"/>
+      <c r="E34" s="182"/>
+      <c r="F34" s="183"/>
+      <c r="G34" s="184"/>
+      <c r="H34" s="185"/>
+      <c r="I34" s="185"/>
+      <c r="J34" s="184"/>
+      <c r="K34" s="184"/>
+      <c r="L34" s="185"/>
+      <c r="M34" s="184"/>
+      <c r="N34" s="184"/>
+      <c r="O34" s="185"/>
+      <c r="P34" s="184"/>
+      <c r="Q34" s="184"/>
+      <c r="R34" s="185"/>
+      <c r="S34" s="184"/>
+      <c r="T34" s="184"/>
+      <c r="U34" s="185"/>
+      <c r="V34" s="184"/>
+      <c r="W34" s="184"/>
+      <c r="X34" s="185"/>
+      <c r="Y34" s="184"/>
+      <c r="Z34" s="184"/>
+      <c r="AA34" s="185"/>
+      <c r="AB34" s="185"/>
     </row>
     <row r="35" spans="1:28" ht="25.5" customHeight="1">
       <c r="A35" s="2" t="s">

</xml_diff>